<commit_message>
se agrego cambios en descargar plantilla de profesores
</commit_message>
<xml_diff>
--- a/schedule-management-backend/src/main/resources/files/templates/plantilla_profesores.xlsx
+++ b/schedule-management-backend/src/main/resources/files/templates/plantilla_profesores.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvarodanieleraso/Desktop/proyecto_1_universidad/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvarodanieleraso/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F60ABA0-B385-104A-A117-6F5A3B555F73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3C16E7-9170-3A4D-BF21-8B5D6458E34F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14380" xr2:uid="{9F743AE1-943A-2A49-89B3-AEBDF22ECA2F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="PROFESORES" sheetId="1" r:id="rId1"/>
+    <sheet name="DEPARTAMENTOS" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Nombre Completo</t>
   </si>
@@ -43,12 +44,18 @@
   <si>
     <t>departamento</t>
   </si>
+  <si>
+    <t>Codigo</t>
+  </si>
+  <si>
+    <t>Nombre departamento</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -65,19 +72,32 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="1"/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -107,12 +127,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -429,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52A916D4-78A8-1140-9F07-C2DA05A9C98D}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -444,15 +471,627 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="2"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="2"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="2"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="2"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="2"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="2"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="2"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="2"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="2"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="2"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="2"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="2"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="2"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="2"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="2"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="2"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="2"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="2"/>
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="2"/>
+      <c r="B77" s="2"/>
+      <c r="C77" s="2"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="2"/>
+      <c r="B78" s="2"/>
+      <c r="C78" s="2"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="2"/>
+      <c r="B79" s="2"/>
+      <c r="C79" s="2"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="2"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="2"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="2"/>
+      <c r="B81" s="2"/>
+      <c r="C81" s="2"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="2"/>
+      <c r="B82" s="2"/>
+      <c r="C82" s="2"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" s="2"/>
+      <c r="B83" s="2"/>
+      <c r="C83" s="2"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" s="2"/>
+      <c r="B84" s="2"/>
+      <c r="C84" s="2"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="2"/>
+      <c r="B85" s="2"/>
+      <c r="C85" s="2"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="2"/>
+      <c r="B86" s="2"/>
+      <c r="C86" s="2"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="2"/>
+      <c r="B87" s="2"/>
+      <c r="C87" s="2"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" s="2"/>
+      <c r="B88" s="2"/>
+      <c r="C88" s="2"/>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" s="2"/>
+      <c r="B89" s="2"/>
+      <c r="C89" s="2"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" s="2"/>
+      <c r="B90" s="2"/>
+      <c r="C90" s="2"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" s="2"/>
+      <c r="B91" s="2"/>
+      <c r="C91" s="2"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" s="2"/>
+      <c r="B92" s="2"/>
+      <c r="C92" s="2"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" s="2"/>
+      <c r="B93" s="2"/>
+      <c r="C93" s="2"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" s="2"/>
+      <c r="B94" s="2"/>
+      <c r="C94" s="2"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" s="2"/>
+      <c r="B95" s="2"/>
+      <c r="C95" s="2"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" s="2"/>
+      <c r="B96" s="2"/>
+      <c r="C96" s="2"/>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" s="2"/>
+      <c r="B97" s="2"/>
+      <c r="C97" s="2"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" s="2"/>
+      <c r="B98" s="2"/>
+      <c r="C98" s="2"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" s="2"/>
+      <c r="B99" s="2"/>
+      <c r="C99" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C9663AD9-C5C5-2C4B-8620-FA61463264DD}">
+          <x14:formula1>
+            <xm:f>DEPARTAMENTOS!$B$2:$B$22</xm:f>
+          </x14:formula1>
+          <xm:sqref>C3:C99 C2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{635D4556-FAFE-1D4A-9C80-C7360EF64A33}">
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>